<commit_message>
add buffer for copy bulk
</commit_message>
<xml_diff>
--- a/benchmarking_read_parquet.xlsx
+++ b/benchmarking_read_parquet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/endangrukmana/Downloads/Frontend/parquet_py/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65BE6B0-0CCD-0144-BC96-7141F25F9285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A678828E-1FF1-3B46-9960-14E4F54500D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16540" xr2:uid="{47DC46F4-9741-D24A-99FE-415648C3D6DA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>BENCHMARK READ DATA PARQUET</t>
   </si>
@@ -66,6 +66,33 @@
   </si>
   <si>
     <t>avg 950 MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> split per 10 files,extract with read_parquet, write to csv, and manual query to copy from csv</t>
+  </si>
+  <si>
+    <t>397 s</t>
+  </si>
+  <si>
+    <t>avg 270 mb</t>
+  </si>
+  <si>
+    <t>to_csv loop all file</t>
+  </si>
+  <si>
+    <t>avg 350 mb</t>
+  </si>
+  <si>
+    <t>write manual to csv</t>
+  </si>
+  <si>
+    <t>376 s</t>
+  </si>
+  <si>
+    <t>avg 300 mb</t>
+  </si>
+  <si>
+    <t>294 s</t>
   </si>
 </sst>
 </file>
@@ -107,10 +134,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,51 +453,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A3D528-B3B4-684F-9CFC-48586EE2B578}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -495,6 +522,48 @@
       </c>
       <c r="G3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>156</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>156</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>